<commit_message>
extract data from excel for and map appropraite IDs for tags of the products
</commit_message>
<xml_diff>
--- a/midas_products.xlsx
+++ b/midas_products.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\extract-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arif\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2641" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2641" uniqueCount="424">
   <si>
     <t>Category</t>
   </si>
@@ -406,9 +406,6 @@
   </si>
   <si>
     <t>Polyester-110</t>
-  </si>
-  <si>
-    <t>Overalls</t>
   </si>
   <si>
     <t>Water-repellent, lightweight, breathable, reflective 
@@ -880,9 +877,6 @@
     <t>Angola Trousers</t>
   </si>
   <si>
-    <t>Trousers</t>
-  </si>
-  <si>
     <t>high abrasion resistance</t>
   </si>
   <si>
@@ -1134,9 +1128,6 @@
     <t>GRS recycled Polyester</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventx Safety Windbreaker Jacket </t>
-  </si>
-  <si>
     <t>segmented reflective, breathable, Waterproof</t>
   </si>
   <si>
@@ -1155,6 +1146,9 @@
     <t>polyester, spandex</t>
   </si>
   <si>
+    <t xml:space="preserve">DWR Flexi Force Jacket </t>
+  </si>
+  <si>
     <t>NOVA Recycled Fleece Jacket</t>
   </si>
   <si>
@@ -1234,9 +1228,6 @@
   </si>
   <si>
     <t>BCI Cotton, Recycled Polyester fleece</t>
-  </si>
-  <si>
-    <t>Sustainable-work Jacket</t>
   </si>
   <si>
     <t>Cotton, Linen</t>
@@ -1363,22 +1354,25 @@
     <t>INCOMBUSTIBLE ALPHA</t>
   </si>
   <si>
-    <t>CLASSIC SERVICES PANTS</t>
-  </si>
-  <si>
-    <t>DURO 2TONE INDUSTRIAL PANT</t>
-  </si>
-  <si>
-    <t>DWR FLEXI FORCE JACKET</t>
+    <t xml:space="preserve"> NYCO TOUGH-INDUSTRIAL JACKET</t>
+  </si>
+  <si>
+    <t>HI-VIS ATHENA JACKET</t>
+  </si>
+  <si>
+    <t>SUSTAINABLE-WORK JACKET</t>
+  </si>
+  <si>
+    <t>VENTX SAFETY WINDBREAKER JACKET</t>
+  </si>
+  <si>
+    <t>Classic Services Pants</t>
   </si>
   <si>
     <t>FR ANTISTATIC BALACLAVA-GREY WHITE</t>
   </si>
   <si>
-    <t>NYCO TOUGH-INDUSTRIAL JACKET</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> HI-VIS ATHENA JACKET</t>
+    <t>Duro 2Tone Industrial Pant</t>
   </si>
 </sst>
 </file>
@@ -1765,13 +1759,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
@@ -2685,7 +2679,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
@@ -2759,7 +2753,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>
@@ -3055,7 +3049,7 @@
         <v>61</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D19" t="s">
         <v>49</v>
@@ -3277,7 +3271,7 @@
         <v>61</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
@@ -3425,7 +3419,7 @@
         <v>61</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -3499,7 +3493,7 @@
         <v>61</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D25" t="s">
         <v>111</v>
@@ -3573,7 +3567,7 @@
         <v>61</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D26" t="s">
         <v>115</v>
@@ -3795,19 +3789,19 @@
         <v>61</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>259</v>
       </c>
       <c r="E29" t="s">
         <v>112</v>
       </c>
       <c r="F29" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" t="s">
         <v>124</v>
-      </c>
-      <c r="G29" t="s">
-        <v>125</v>
       </c>
       <c r="I29" t="s">
         <v>27</v>
@@ -3866,31 +3860,31 @@
         <v>61</v>
       </c>
       <c r="C30" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" t="s">
         <v>126</v>
-      </c>
-      <c r="D30" t="s">
-        <v>127</v>
       </c>
       <c r="E30" t="s">
         <v>112</v>
       </c>
       <c r="F30" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="H30" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="I30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30" t="s">
         <v>130</v>
-      </c>
-      <c r="I30" t="s">
-        <v>27</v>
-      </c>
-      <c r="J30" t="s">
-        <v>27</v>
-      </c>
-      <c r="K30" t="s">
-        <v>131</v>
       </c>
       <c r="L30" t="s">
         <v>27</v>
@@ -3940,7 +3934,7 @@
         <v>61</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D31" t="s">
         <v>49</v>
@@ -3949,7 +3943,7 @@
         <v>27</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G31" t="s">
         <v>38</v>
@@ -3982,7 +3976,7 @@
         <v>27</v>
       </c>
       <c r="Q31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R31" t="s">
         <v>27</v>
@@ -4011,40 +4005,40 @@
         <v>29</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" t="s">
         <v>136</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="F32" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="G32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" t="s">
+        <v>27</v>
+      </c>
+      <c r="K32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="G32" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" t="s">
-        <v>27</v>
-      </c>
-      <c r="I32" t="s">
-        <v>27</v>
-      </c>
-      <c r="J32" t="s">
-        <v>27</v>
-      </c>
-      <c r="K32" t="s">
-        <v>27</v>
-      </c>
-      <c r="L32" t="s">
-        <v>27</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="N32" t="s">
         <v>27</v>
@@ -4085,40 +4079,40 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D33" t="s">
         <v>26</v>
       </c>
       <c r="E33" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="G33" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="G33" t="s">
-        <v>27</v>
-      </c>
-      <c r="H33" t="s">
-        <v>27</v>
-      </c>
-      <c r="I33" t="s">
-        <v>27</v>
-      </c>
-      <c r="J33" t="s">
-        <v>27</v>
-      </c>
-      <c r="K33" t="s">
-        <v>27</v>
-      </c>
-      <c r="L33" t="s">
-        <v>27</v>
-      </c>
-      <c r="M33" s="8" t="s">
-        <v>144</v>
       </c>
       <c r="N33" t="s">
         <v>27</v>
@@ -4159,40 +4153,40 @@
         <v>31</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C34" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" t="s">
         <v>145</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="G34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J34" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" t="s">
+        <v>27</v>
+      </c>
+      <c r="L34" t="s">
+        <v>27</v>
+      </c>
+      <c r="M34" t="s">
         <v>148</v>
-      </c>
-      <c r="G34" t="s">
-        <v>27</v>
-      </c>
-      <c r="H34" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" t="s">
-        <v>27</v>
-      </c>
-      <c r="J34" t="s">
-        <v>27</v>
-      </c>
-      <c r="K34" t="s">
-        <v>27</v>
-      </c>
-      <c r="L34" t="s">
-        <v>27</v>
-      </c>
-      <c r="M34" t="s">
-        <v>149</v>
       </c>
       <c r="N34" t="s">
         <v>27</v>
@@ -4233,25 +4227,25 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D35" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="G35" t="s">
         <v>152</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>154</v>
       </c>
       <c r="I35" t="s">
         <v>27</v>
@@ -4307,55 +4301,55 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="D36" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F36" s="8" t="s">
+      <c r="G36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="G36" t="s">
-        <v>27</v>
-      </c>
-      <c r="H36" s="8" t="s">
+      <c r="I36" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" t="s">
         <v>157</v>
       </c>
-      <c r="I36" t="s">
-        <v>27</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
+        <v>27</v>
+      </c>
+      <c r="L36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M36" t="s">
+        <v>27</v>
+      </c>
+      <c r="N36" t="s">
+        <v>27</v>
+      </c>
+      <c r="O36" t="s">
+        <v>27</v>
+      </c>
+      <c r="P36" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>27</v>
+      </c>
+      <c r="R36" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="K36" t="s">
-        <v>27</v>
-      </c>
-      <c r="L36" t="s">
-        <v>27</v>
-      </c>
-      <c r="M36" t="s">
-        <v>27</v>
-      </c>
-      <c r="N36" t="s">
-        <v>27</v>
-      </c>
-      <c r="O36" t="s">
-        <v>27</v>
-      </c>
-      <c r="P36" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>27</v>
-      </c>
-      <c r="R36" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="S36" t="s">
         <v>27</v>
@@ -4381,25 +4375,25 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C37" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D37" t="s">
-        <v>146</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F37" s="8" t="s">
+      <c r="G37" t="s">
         <v>161</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>163</v>
       </c>
       <c r="I37" t="s">
         <v>27</v>
@@ -4455,25 +4449,25 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C38" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D38" t="s">
         <v>164</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="H38" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>169</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>27</v>
@@ -4529,22 +4523,22 @@
         <v>36</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C39" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D39" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D39" t="s">
-        <v>165</v>
-      </c>
-      <c r="E39" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="G39" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>27</v>
@@ -4603,22 +4597,22 @@
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C40" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" t="s">
+        <v>164</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="D40" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="G40" t="s">
         <v>176</v>
-      </c>
-      <c r="G40" t="s">
-        <v>177</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>27</v>
@@ -4677,40 +4671,40 @@
         <v>38</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E41" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F41" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="G41" t="s">
+        <v>27</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" t="s">
+        <v>27</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K41" t="s">
+        <v>27</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M41" t="s">
         <v>179</v>
-      </c>
-      <c r="G41" t="s">
-        <v>27</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I41" t="s">
-        <v>27</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K41" t="s">
-        <v>27</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M41" t="s">
-        <v>180</v>
       </c>
       <c r="N41" s="8" t="s">
         <v>27</v>
@@ -4751,20 +4745,20 @@
         <v>39</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C42" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D42" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D42" t="s">
-        <v>137</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>182</v>
-      </c>
       <c r="G42" t="s">
         <v>27</v>
       </c>
@@ -4784,7 +4778,7 @@
         <v>27</v>
       </c>
       <c r="M42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N42" s="8" t="s">
         <v>27</v>
@@ -4825,46 +4819,46 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C43" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" t="s">
+        <v>136</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D43" t="s">
-        <v>137</v>
-      </c>
-      <c r="E43" s="8" t="s">
+      <c r="F43" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="G43" t="s">
         <v>185</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I43" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="H43" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I43" t="s">
-        <v>27</v>
-      </c>
-      <c r="J43" s="8" t="s">
+      <c r="K43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O43" t="s">
         <v>187</v>
-      </c>
-      <c r="K43" t="s">
-        <v>27</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M43" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N43" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O43" t="s">
-        <v>188</v>
       </c>
       <c r="P43" s="8" t="s">
         <v>27</v>
@@ -4899,31 +4893,31 @@
         <v>41</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D44" t="s">
         <v>26</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F44" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G44" t="s">
+        <v>148</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I44" t="s">
+        <v>27</v>
+      </c>
+      <c r="J44" s="8" t="s">
         <v>190</v>
-      </c>
-      <c r="G44" t="s">
-        <v>149</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I44" t="s">
-        <v>27</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>191</v>
       </c>
       <c r="K44" t="s">
         <v>27</v>
@@ -4973,31 +4967,31 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C45" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D45" t="s">
+        <v>126</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="D45" t="s">
-        <v>127</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F45" s="8" t="s">
+      <c r="G45" t="s">
         <v>193</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I45" t="s">
+        <v>27</v>
+      </c>
+      <c r="J45" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I45" t="s">
-        <v>27</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="K45" t="s">
         <v>27</v>
@@ -5047,40 +5041,40 @@
         <v>43</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C46" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D46" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="D46" t="s">
-        <v>137</v>
-      </c>
-      <c r="E46" s="8" t="s">
+      <c r="F46" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="G46" t="s">
+        <v>27</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46" t="s">
+        <v>27</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" t="s">
+        <v>27</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="G46" t="s">
-        <v>27</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I46" t="s">
-        <v>27</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K46" t="s">
-        <v>27</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M46" s="8" t="s">
-        <v>199</v>
       </c>
       <c r="N46" s="8" t="s">
         <v>27</v>
@@ -5121,40 +5115,40 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C47" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D47" t="s">
+        <v>164</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G47" t="s">
+        <v>27</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I47" t="s">
+        <v>27</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K47" t="s">
+        <v>27</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M47" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="D47" t="s">
-        <v>165</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="G47" t="s">
-        <v>27</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I47" t="s">
-        <v>27</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K47" t="s">
-        <v>27</v>
-      </c>
-      <c r="L47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M47" s="8" t="s">
-        <v>201</v>
       </c>
       <c r="N47" s="8" t="s">
         <v>27</v>
@@ -5195,22 +5189,22 @@
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C48" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D48" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F48" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D48" t="s">
-        <v>137</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F48" s="8" t="s">
+      <c r="G48" t="s">
         <v>203</v>
-      </c>
-      <c r="G48" t="s">
-        <v>204</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>27</v>
@@ -5269,22 +5263,22 @@
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C49" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D49" t="s">
         <v>205</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="F49" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G49" t="s">
         <v>207</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G49" t="s">
-        <v>208</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>27</v>
@@ -5343,22 +5337,22 @@
         <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E50" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G50" t="s">
         <v>209</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G50" t="s">
-        <v>210</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>27</v>
@@ -5417,23 +5411,23 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
+        <v>210</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>212</v>
       </c>
       <c r="D51" t="s">
         <v>87</v>
       </c>
       <c r="E51" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F51" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="G51" t="s">
         <v>214</v>
       </c>
-      <c r="G51" t="s">
-        <v>215</v>
-      </c>
       <c r="H51" s="8" t="s">
         <v>27</v>
       </c>
@@ -5468,7 +5462,7 @@
         <v>27</v>
       </c>
       <c r="S51" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T51" s="8" t="s">
         <v>27</v>
@@ -5491,10 +5485,10 @@
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D52" t="s">
         <v>26</v>
@@ -5503,19 +5497,19 @@
         <v>27</v>
       </c>
       <c r="F52" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G52" t="s">
         <v>217</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="I52" t="s">
         <v>219</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="J52" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="K52" t="s">
         <v>27</v>
@@ -5565,10 +5559,10 @@
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D53" t="s">
         <v>26</v>
@@ -5577,19 +5571,19 @@
         <v>27</v>
       </c>
       <c r="F53" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="G53" t="s">
         <v>223</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I53" t="s">
+        <v>27</v>
+      </c>
+      <c r="J53" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I53" t="s">
-        <v>27</v>
-      </c>
-      <c r="J53" s="8" t="s">
-        <v>225</v>
       </c>
       <c r="K53" t="s">
         <v>27</v>
@@ -5639,25 +5633,25 @@
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C54" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D54" t="s">
+        <v>164</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="D54" t="s">
-        <v>165</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F54" s="8" t="s">
+      <c r="G54" t="s">
         <v>227</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" s="8" t="s">
         <v>228</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>229</v>
       </c>
       <c r="I54" t="s">
         <v>27</v>
@@ -5713,10 +5707,10 @@
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D55" t="s">
         <v>26</v>
@@ -5725,19 +5719,19 @@
         <v>27</v>
       </c>
       <c r="F55" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="G55" t="s">
         <v>231</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="I55" t="s">
+        <v>27</v>
+      </c>
+      <c r="J55" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="I55" t="s">
-        <v>27</v>
-      </c>
-      <c r="J55" s="8" t="s">
-        <v>234</v>
       </c>
       <c r="K55" t="s">
         <v>27</v>
@@ -5787,25 +5781,25 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C56" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D56" t="s">
+        <v>164</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="G56" t="s">
         <v>235</v>
       </c>
-      <c r="D56" t="s">
-        <v>165</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="H56" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>237</v>
       </c>
       <c r="I56" t="s">
         <v>27</v>
@@ -5861,25 +5855,25 @@
         <v>54</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C57" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" t="s">
+        <v>164</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="D57" t="s">
-        <v>165</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F57" s="8" t="s">
+      <c r="G57" t="s">
         <v>239</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>241</v>
       </c>
       <c r="I57" t="s">
         <v>27</v>
@@ -5935,25 +5929,25 @@
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F58" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="G58" t="s">
         <v>242</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="I58" t="s">
         <v>27</v>
@@ -6009,10 +6003,10 @@
         <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D59" t="s">
         <v>87</v>
@@ -6021,49 +6015,49 @@
         <v>27</v>
       </c>
       <c r="F59" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="G59" t="s">
         <v>246</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="H59" s="8" t="s">
+      <c r="I59" t="s">
+        <v>27</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K59" t="s">
+        <v>27</v>
+      </c>
+      <c r="L59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O59" t="s">
+        <v>27</v>
+      </c>
+      <c r="P59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T59" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="I59" t="s">
-        <v>27</v>
-      </c>
-      <c r="J59" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K59" t="s">
-        <v>27</v>
-      </c>
-      <c r="L59" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M59" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N59" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O59" t="s">
-        <v>27</v>
-      </c>
-      <c r="P59" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q59" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R59" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S59" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T59" s="8" t="s">
-        <v>249</v>
       </c>
       <c r="U59" s="8" t="s">
         <v>27</v>
@@ -6083,10 +6077,10 @@
         <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D60" t="s">
         <v>26</v>
@@ -6095,10 +6089,10 @@
         <v>27</v>
       </c>
       <c r="F60" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="G60" t="s">
         <v>251</v>
-      </c>
-      <c r="G60" t="s">
-        <v>252</v>
       </c>
       <c r="H60" s="8" t="s">
         <v>27</v>
@@ -6157,22 +6151,22 @@
         <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C61" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D61" t="s">
+        <v>136</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F61" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="D61" t="s">
-        <v>137</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>254</v>
-      </c>
       <c r="G61" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H61" s="8" t="s">
         <v>27</v>
@@ -6231,22 +6225,22 @@
         <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C62" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D62" t="s">
         <v>255</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F62" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="E62" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F62" s="8" t="s">
+      <c r="G62" t="s">
         <v>257</v>
-      </c>
-      <c r="G62" t="s">
-        <v>258</v>
       </c>
       <c r="H62" s="8" t="s">
         <v>27</v>
@@ -6305,20 +6299,20 @@
         <v>60</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C63" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D63" t="s">
         <v>259</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F63" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="E63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>261</v>
-      </c>
       <c r="G63" s="8" t="s">
         <v>27</v>
       </c>
@@ -6338,7 +6332,7 @@
         <v>27</v>
       </c>
       <c r="M63" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N63" s="8" t="s">
         <v>27</v>
@@ -6379,40 +6373,40 @@
         <v>61</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C64" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D64" t="s">
+        <v>87</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="D64" t="s">
+      <c r="G64" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" t="s">
+        <v>27</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K64" t="s">
+        <v>27</v>
+      </c>
+      <c r="L64" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M64" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H64" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" t="s">
-        <v>27</v>
-      </c>
-      <c r="J64" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K64" t="s">
-        <v>27</v>
-      </c>
-      <c r="L64" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M64" s="8" t="s">
-        <v>265</v>
       </c>
       <c r="N64" s="8" t="s">
         <v>27</v>
@@ -6453,10 +6447,10 @@
         <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="D65" t="s">
         <v>26</v>
@@ -6465,7 +6459,7 @@
         <v>27</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G65" s="8" t="s">
         <v>27</v>
@@ -6486,7 +6480,7 @@
         <v>27</v>
       </c>
       <c r="M65" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N65" s="8" t="s">
         <v>27</v>
@@ -6527,10 +6521,10 @@
         <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D66" t="s">
         <v>26</v>
@@ -6539,10 +6533,10 @@
         <v>27</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H66" s="8" t="s">
         <v>27</v>
@@ -6601,46 +6595,46 @@
         <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C67" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D67" t="s">
+        <v>164</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="G67" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="D67" t="s">
-        <v>165</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F67" s="8" t="s">
+      <c r="H67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I67" t="s">
+        <v>27</v>
+      </c>
+      <c r="J67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K67" t="s">
+        <v>27</v>
+      </c>
+      <c r="L67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O67" s="8" t="s">
         <v>271</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="H67" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I67" t="s">
-        <v>27</v>
-      </c>
-      <c r="J67" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K67" t="s">
-        <v>27</v>
-      </c>
-      <c r="L67" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M67" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N67" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O67" s="8" t="s">
-        <v>273</v>
       </c>
       <c r="P67" s="8" t="s">
         <v>27</v>
@@ -6675,10 +6669,10 @@
         <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D68" t="s">
         <v>26</v>
@@ -6687,52 +6681,52 @@
         <v>27</v>
       </c>
       <c r="F68" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" t="s">
+        <v>27</v>
+      </c>
+      <c r="J68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K68" t="s">
+        <v>27</v>
+      </c>
+      <c r="L68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U68" s="8" t="s">
         <v>275</v>
-      </c>
-      <c r="G68" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="H68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I68" t="s">
-        <v>27</v>
-      </c>
-      <c r="J68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K68" t="s">
-        <v>27</v>
-      </c>
-      <c r="L68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T68" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="U68" s="8" t="s">
-        <v>277</v>
       </c>
       <c r="V68" s="8" t="s">
         <v>27</v>
@@ -6749,40 +6743,40 @@
         <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C69" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D69" t="s">
+        <v>136</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I69" t="s">
+        <v>27</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K69" t="s">
+        <v>27</v>
+      </c>
+      <c r="L69" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M69" s="8" t="s">
         <v>278</v>
-      </c>
-      <c r="D69" t="s">
-        <v>137</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="G69" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H69" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I69" t="s">
-        <v>27</v>
-      </c>
-      <c r="J69" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K69" t="s">
-        <v>27</v>
-      </c>
-      <c r="L69" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M69" s="8" t="s">
-        <v>280</v>
       </c>
       <c r="N69" s="8" t="s">
         <v>27</v>
@@ -6823,10 +6817,10 @@
         <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D70" t="s">
         <v>49</v>
@@ -6835,7 +6829,7 @@
         <v>27</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G70" s="8" t="s">
         <v>27</v>
@@ -6856,7 +6850,7 @@
         <v>27</v>
       </c>
       <c r="M70" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="N70" s="8" t="s">
         <v>27</v>
@@ -6897,64 +6891,64 @@
         <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C71" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D71" t="s">
+        <v>87</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="G71" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="D71" t="s">
-        <v>263</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F71" s="8" t="s">
+      <c r="H71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T71" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U71" s="8" t="s">
         <v>284</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="H71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="U71" s="8" t="s">
-        <v>286</v>
       </c>
       <c r="V71" s="8" t="s">
         <v>27</v>
@@ -6971,19 +6965,19 @@
         <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D72" t="s">
-        <v>263</v>
+        <v>87</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G72" s="8" t="s">
         <v>79</v>
@@ -7045,22 +7039,22 @@
         <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C73" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D73" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="G73" s="8" t="s">
         <v>289</v>
-      </c>
-      <c r="D73" t="s">
-        <v>165</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="G73" s="8" t="s">
-        <v>291</v>
       </c>
       <c r="H73" s="8" t="s">
         <v>27</v>
@@ -7119,22 +7113,22 @@
         <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C74" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D74" t="s">
+        <v>87</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="G74" s="8" t="s">
         <v>292</v>
-      </c>
-      <c r="D74" t="s">
-        <v>263</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F74" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="G74" s="8" t="s">
-        <v>294</v>
       </c>
       <c r="H74" s="8" t="s">
         <v>92</v>
@@ -7193,22 +7187,22 @@
         <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C75" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D75" t="s">
+        <v>164</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="G75" s="8" t="s">
         <v>295</v>
-      </c>
-      <c r="D75" t="s">
-        <v>165</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F75" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="G75" s="8" t="s">
-        <v>297</v>
       </c>
       <c r="H75" s="8" t="s">
         <v>27</v>
@@ -7267,25 +7261,25 @@
         <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D76" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G76" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="H76" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="H76" s="8" t="s">
-        <v>299</v>
       </c>
       <c r="I76" s="8" t="s">
         <v>27</v>
@@ -7341,10 +7335,10 @@
         <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D77" t="s">
         <v>26</v>
@@ -7353,7 +7347,7 @@
         <v>27</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G77" s="8" t="s">
         <v>38</v>
@@ -7365,7 +7359,7 @@
         <v>27</v>
       </c>
       <c r="J77" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K77" s="8" t="s">
         <v>38</v>
@@ -7415,10 +7409,10 @@
         <v>75</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D78" t="s">
         <v>26</v>
@@ -7427,50 +7421,50 @@
         <v>27</v>
       </c>
       <c r="F78" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="G78" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="H78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T78" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="G78" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="H78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T78" s="8" t="s">
-        <v>307</v>
-      </c>
       <c r="U78" s="8" t="s">
         <v>27</v>
       </c>
@@ -7484,15 +7478,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>76</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D79" t="s">
         <v>26</v>
@@ -7501,10 +7495,10 @@
         <v>27</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G79" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H79" s="8" t="s">
         <v>27</v>
@@ -7563,10 +7557,10 @@
         <v>77</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D80" t="s">
         <v>26</v>
@@ -7575,7 +7569,7 @@
         <v>27</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G80" s="8" t="s">
         <v>110</v>
@@ -7587,7 +7581,7 @@
         <v>27</v>
       </c>
       <c r="J80" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K80" s="8" t="s">
         <v>27</v>
@@ -7637,10 +7631,10 @@
         <v>78</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D81" t="s">
         <v>26</v>
@@ -7649,13 +7643,13 @@
         <v>27</v>
       </c>
       <c r="F81" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="H81" s="8" t="s">
         <v>314</v>
-      </c>
-      <c r="G81" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>316</v>
       </c>
       <c r="I81" s="8" t="s">
         <v>27</v>
@@ -7711,22 +7705,22 @@
         <v>79</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C82" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D82" t="s">
+        <v>164</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="G82" s="8" t="s">
         <v>317</v>
-      </c>
-      <c r="D82" t="s">
-        <v>165</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="G82" s="8" t="s">
-        <v>319</v>
       </c>
       <c r="H82" s="8" t="s">
         <v>27</v>
@@ -7785,28 +7779,28 @@
         <v>80</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C83" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D83" t="s">
+        <v>164</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="G83" s="8" t="s">
         <v>320</v>
-      </c>
-      <c r="D83" t="s">
-        <v>165</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="G83" s="8" t="s">
-        <v>322</v>
       </c>
       <c r="H83" s="8" t="s">
         <v>43</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J83" s="8" t="s">
         <v>27</v>
@@ -7859,40 +7853,40 @@
         <v>81</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C84" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D84" t="s">
+        <v>164</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I84" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J84" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K84" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L84" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M84" s="8" t="s">
         <v>324</v>
-      </c>
-      <c r="D84" t="s">
-        <v>165</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H84" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I84" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J84" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K84" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L84" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M84" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="N84" s="8" t="s">
         <v>27</v>
@@ -7933,10 +7927,10 @@
         <v>82</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D85" t="s">
         <v>26</v>
@@ -7945,52 +7939,52 @@
         <v>27</v>
       </c>
       <c r="F85" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="G85" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="H85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J85" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="G85" s="8" t="s">
+      <c r="K85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U85" s="8" t="s">
         <v>329</v>
-      </c>
-      <c r="H85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J85" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="K85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T85" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="U85" s="8" t="s">
-        <v>331</v>
       </c>
       <c r="V85" s="8" t="s">
         <v>27</v>
@@ -8007,10 +8001,10 @@
         <v>83</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D86" t="s">
         <v>26</v>
@@ -8019,7 +8013,7 @@
         <v>27</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G86" s="8" t="s">
         <v>27</v>
@@ -8040,7 +8034,7 @@
         <v>27</v>
       </c>
       <c r="M86" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N86" s="8" t="s">
         <v>27</v>
@@ -8081,40 +8075,40 @@
         <v>84</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D87" t="s">
         <v>26</v>
       </c>
       <c r="E87" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I87" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J87" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K87" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L87" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M87" s="8" t="s">
         <v>336</v>
-      </c>
-      <c r="F87" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="G87" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H87" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I87" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J87" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K87" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L87" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M87" s="8" t="s">
-        <v>338</v>
       </c>
       <c r="N87" s="8" t="s">
         <v>27</v>
@@ -8155,10 +8149,10 @@
         <v>85</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D88" t="s">
         <v>26</v>
@@ -8167,7 +8161,7 @@
         <v>27</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G88" s="8" t="s">
         <v>32</v>
@@ -8224,15 +8218,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>86</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D89" t="s">
         <v>26</v>
@@ -8241,7 +8235,7 @@
         <v>27</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G89" s="8" t="s">
         <v>38</v>
@@ -8289,7 +8283,7 @@
         <v>27</v>
       </c>
       <c r="V89" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="W89" s="8" t="s">
         <v>27</v>
@@ -8303,10 +8297,10 @@
         <v>87</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>344</v>
+        <v>420</v>
       </c>
       <c r="D90" t="s">
         <v>26</v>
@@ -8315,10 +8309,10 @@
         <v>27</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H90" s="8" t="s">
         <v>27</v>
@@ -8366,7 +8360,7 @@
         <v>27</v>
       </c>
       <c r="W90" s="8" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="X90" s="8" t="s">
         <v>27</v>
@@ -8377,10 +8371,10 @@
         <v>88</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D91" t="s">
         <v>26</v>
@@ -8389,13 +8383,13 @@
         <v>27</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I91" s="8" t="s">
         <v>27</v>
@@ -8451,10 +8445,10 @@
         <v>89</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>422</v>
+        <v>348</v>
       </c>
       <c r="D92" t="s">
         <v>26</v>
@@ -8520,15 +8514,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>90</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D93" t="s">
         <v>26</v>
@@ -8537,10 +8531,10 @@
         <v>27</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H93" s="8" t="s">
         <v>27</v>
@@ -8594,15 +8588,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>91</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D94" t="s">
         <v>26</v>
@@ -8611,10 +8605,10 @@
         <v>27</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H94" s="8" t="s">
         <v>27</v>
@@ -8673,10 +8667,10 @@
         <v>92</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D95" t="s">
         <v>26</v>
@@ -8685,13 +8679,13 @@
         <v>27</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G95" s="8" t="s">
         <v>92</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>27</v>
@@ -8700,7 +8694,7 @@
         <v>27</v>
       </c>
       <c r="K95" s="8" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L95" s="8" t="s">
         <v>27</v>
@@ -8747,10 +8741,10 @@
         <v>93</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D96" t="s">
         <v>26</v>
@@ -8759,10 +8753,10 @@
         <v>27</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H96" s="8" t="s">
         <v>27</v>
@@ -8821,10 +8815,10 @@
         <v>94</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D97" t="s">
         <v>26</v>
@@ -8833,7 +8827,7 @@
         <v>27</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>38</v>
@@ -8881,7 +8875,7 @@
         <v>27</v>
       </c>
       <c r="V97" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="W97" s="8" t="s">
         <v>27</v>
@@ -8895,22 +8889,22 @@
         <v>95</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C98" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D98" t="s">
+        <v>136</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="G98" s="8" t="s">
         <v>363</v>
-      </c>
-      <c r="D98" t="s">
-        <v>137</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F98" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="G98" s="8" t="s">
-        <v>365</v>
       </c>
       <c r="H98" s="8" t="s">
         <v>27</v>
@@ -8969,22 +8963,22 @@
         <v>96</v>
       </c>
       <c r="B99" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D99" t="s">
+        <v>164</v>
+      </c>
+      <c r="E99" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F99" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="G99" s="8" t="s">
         <v>367</v>
-      </c>
-      <c r="D99" t="s">
-        <v>165</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F99" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="G99" s="8" t="s">
-        <v>369</v>
       </c>
       <c r="H99" s="8" t="s">
         <v>27</v>
@@ -9043,22 +9037,22 @@
         <v>97</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D100" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H100" s="8" t="s">
         <v>27</v>
@@ -9117,10 +9111,10 @@
         <v>98</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D101" t="s">
         <v>26</v>
@@ -9129,10 +9123,10 @@
         <v>27</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H101" s="8" t="s">
         <v>27</v>
@@ -9191,25 +9185,25 @@
         <v>99</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C102" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="D102" t="s">
+        <v>87</v>
+      </c>
+      <c r="E102" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F102" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="G102" t="s">
         <v>375</v>
       </c>
-      <c r="D102" t="s">
-        <v>263</v>
-      </c>
-      <c r="E102" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F102" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="G102" t="s">
-        <v>377</v>
-      </c>
       <c r="H102" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I102" s="8" t="s">
         <v>27</v>
@@ -9265,10 +9259,10 @@
         <v>100</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>378</v>
+        <v>419</v>
       </c>
       <c r="D103" t="s">
         <v>26</v>
@@ -9277,13 +9271,13 @@
         <v>27</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I103" s="8" t="s">
         <v>27</v>
@@ -9339,10 +9333,10 @@
         <v>101</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D104" t="s">
         <v>111</v>
@@ -9351,7 +9345,7 @@
         <v>27</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G104" s="8" t="s">
         <v>27</v>
@@ -9372,7 +9366,7 @@
         <v>27</v>
       </c>
       <c r="M104" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="N104" s="8" t="s">
         <v>27</v>
@@ -9413,19 +9407,19 @@
         <v>102</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D105" t="s">
-        <v>263</v>
+        <v>87</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G105" s="8" t="s">
         <v>27</v>
@@ -9446,7 +9440,7 @@
         <v>27</v>
       </c>
       <c r="M105" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="N105" s="8" t="s">
         <v>27</v>
@@ -9487,10 +9481,10 @@
         <v>103</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D106" t="s">
         <v>69</v>
@@ -9499,7 +9493,7 @@
         <v>27</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G106" s="8" t="s">
         <v>27</v>
@@ -9520,7 +9514,7 @@
         <v>27</v>
       </c>
       <c r="M106" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="N106" s="8" t="s">
         <v>27</v>
@@ -9561,10 +9555,10 @@
         <v>104</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D107" t="s">
         <v>26</v>
@@ -9573,7 +9567,7 @@
         <v>27</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G107" s="8" t="s">
         <v>27</v>
@@ -9594,7 +9588,7 @@
         <v>27</v>
       </c>
       <c r="M107" s="8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="N107" s="8" t="s">
         <v>27</v>
@@ -9635,22 +9629,22 @@
         <v>105</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D108" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E108" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G108" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H108" s="8" t="s">
         <v>27</v>
@@ -9709,22 +9703,22 @@
         <v>106</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D109" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G109" s="8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="H109" s="8" t="s">
         <v>27</v>
@@ -9783,19 +9777,19 @@
         <v>107</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D110" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G110" s="8" t="s">
         <v>27</v>
@@ -9816,7 +9810,7 @@
         <v>27</v>
       </c>
       <c r="M110" s="8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="N110" s="8" t="s">
         <v>27</v>
@@ -9857,22 +9851,22 @@
         <v>108</v>
       </c>
       <c r="B111" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="D111" t="s">
+        <v>393</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F111" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="G111" s="8" t="s">
         <v>395</v>
-      </c>
-      <c r="D111" t="s">
-        <v>396</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F111" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="G111" s="8" t="s">
-        <v>398</v>
       </c>
       <c r="H111" s="8" t="s">
         <v>27</v>
@@ -9931,22 +9925,22 @@
         <v>109</v>
       </c>
       <c r="B112" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="D112" t="s">
+        <v>393</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F112" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="C112" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="D112" t="s">
-        <v>396</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F112" s="8" t="s">
+      <c r="G112" s="8" t="s">
         <v>397</v>
-      </c>
-      <c r="G112" s="8" t="s">
-        <v>400</v>
       </c>
       <c r="H112" s="8" t="s">
         <v>27</v>
@@ -10005,22 +9999,22 @@
         <v>110</v>
       </c>
       <c r="B113" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="D113" t="s">
+        <v>393</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F113" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="C113" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="D113" t="s">
-        <v>396</v>
-      </c>
-      <c r="E113" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F113" s="8" t="s">
-        <v>397</v>
-      </c>
       <c r="G113" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H113" s="8" t="s">
         <v>27</v>
@@ -10079,10 +10073,10 @@
         <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D114" t="s">
         <v>111</v>
@@ -10091,7 +10085,7 @@
         <v>27</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G114" s="8" t="s">
         <v>27</v>
@@ -10112,7 +10106,7 @@
         <v>27</v>
       </c>
       <c r="M114" s="8" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="N114" s="8" t="s">
         <v>27</v>
@@ -10153,73 +10147,73 @@
         <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C115" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D115" t="s">
+        <v>164</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="V115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="W115" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="X115" s="8" t="s">
         <v>406</v>
-      </c>
-      <c r="D115" t="s">
-        <v>165</v>
-      </c>
-      <c r="E115" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="F115" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="G115" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="H115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="U115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="V115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="W115" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="X115" s="8" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="116" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -10227,22 +10221,22 @@
         <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D116" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G116" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H116" s="8" t="s">
         <v>27</v>
@@ -10293,7 +10287,7 @@
         <v>27</v>
       </c>
       <c r="X116" s="8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -10301,6 +10295,5 @@
     <mergeCell ref="G1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>